<commit_message>
Need help figuring out subfolders with terraform
</commit_message>
<xml_diff>
--- a/deploy-tenant_input_Spreadsheet.xlsx
+++ b/deploy-tenant_input_Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D01617-FD4F-4062-B639-43F2DC011604}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428B6A16-42A7-44EE-B104-208FDAE58CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tenant" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="242">
   <si>
     <t>Type</t>
   </si>
@@ -316,9 +316,6 @@
     <t>leaf201</t>
   </si>
   <si>
-    <t>201</t>
-  </si>
-  <si>
     <t>Routed Interface</t>
   </si>
   <si>
@@ -328,15 +325,9 @@
     <t>Create Interface Policy Groups</t>
   </si>
   <si>
-    <t>1500</t>
-  </si>
-  <si>
     <t>trunk</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>998-999</t>
   </si>
   <si>
@@ -358,18 +349,12 @@
     <t>access</t>
   </si>
   <si>
-    <t>995</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>143c-lab-gw1-Te0/0/4</t>
   </si>
   <si>
-    <t>691</t>
-  </si>
-  <si>
     <t>r143c-netapp01-ct0-vpc</t>
   </si>
   <si>
@@ -478,21 +463,12 @@
     <t>r143b-ucs-b_vpc</t>
   </si>
   <si>
-    <t>142b-oob_vpc</t>
-  </si>
-  <si>
     <t>asgard-leaf_vpc</t>
   </si>
   <si>
     <t>wakanda-leaf_vpc</t>
   </si>
   <si>
-    <t>143-oob_vpc</t>
-  </si>
-  <si>
-    <t>143-dist_vpc</t>
-  </si>
-  <si>
     <t>Eth1-01</t>
   </si>
   <si>
@@ -548,18 +524,6 @@
   </si>
   <si>
     <t>BreakOut Group Name</t>
-  </si>
-  <si>
-    <t>Eth1-1-01</t>
-  </si>
-  <si>
-    <t>Eth1-1-02</t>
-  </si>
-  <si>
-    <t>Eth1-1-03</t>
-  </si>
-  <si>
-    <t>Eth1-1-04</t>
   </si>
   <si>
     <r>
@@ -827,9 +791,6 @@
     <t>dmz_vrf</t>
   </si>
   <si>
-    <t>pod_vrf</t>
-  </si>
-  <si>
     <t>LACP Policy</t>
   </si>
   <si>
@@ -867,13 +828,34 @@
   </si>
   <si>
     <t>Node Id (2 if vpc)</t>
+  </si>
+  <si>
+    <t>r142b-oob_vpc</t>
+  </si>
+  <si>
+    <t>r143-oob_vpc</t>
+  </si>
+  <si>
+    <t>r143-dist_vpc</t>
+  </si>
+  <si>
+    <t>Eth1-01-1</t>
+  </si>
+  <si>
+    <t>Eth1-01-2</t>
+  </si>
+  <si>
+    <t>Eth1-01-3</t>
+  </si>
+  <si>
+    <t>Eth1-01-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1051,6 +1033,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF44546A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1656,7 +1645,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyAlignment="1">
@@ -1722,6 +1711,16 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2"/>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1729,15 +1728,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2" applyAlignment="1">
@@ -1755,6 +1745,15 @@
     <xf numFmtId="0" fontId="3" fillId="34" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="19" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1764,22 +1763,27 @@
     <xf numFmtId="49" fontId="19" fillId="34" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="33" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="33" borderId="8" xfId="2"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="43" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="24" xfId="44" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1831,6 +1835,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF44546A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2167,38 +2176,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="122.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="B2" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2207,16 +2216,16 @@
       <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="30" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="6" t="s">
         <v>52</v>
       </c>
@@ -2232,16 +2241,16 @@
       <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="26" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
       <c r="I4" s="9" t="s">
         <v>53</v>
       </c>
@@ -2257,14 +2266,14 @@
       <c r="B5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="7" t="s">
         <v>54</v>
       </c>
@@ -2276,12 +2285,12 @@
     <row r="6" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -2291,12 +2300,12 @@
     <row r="7" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -2306,12 +2315,12 @@
     <row r="8" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -2321,12 +2330,12 @@
     <row r="9" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -2336,12 +2345,12 @@
     <row r="10" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -2351,12 +2360,12 @@
     <row r="11" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="25"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="29"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
@@ -2366,12 +2375,12 @@
     <row r="12" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -2381,12 +2390,12 @@
     <row r="13" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -2396,12 +2405,12 @@
     <row r="14" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
@@ -2411,12 +2420,12 @@
     <row r="15" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -2426,12 +2435,12 @@
     <row r="16" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
@@ -2441,12 +2450,12 @@
     <row r="17" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -2456,12 +2465,12 @@
     <row r="18" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -2471,12 +2480,12 @@
     <row r="19" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="25"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -2486,12 +2495,12 @@
     <row r="20" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
@@ -2501,12 +2510,12 @@
     <row r="21" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="25"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -2516,12 +2525,12 @@
     <row r="22" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="26"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
@@ -2531,12 +2540,12 @@
     <row r="23" spans="1:13" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="25"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="29"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
@@ -2545,6 +2554,38 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="F6:H6"/>
@@ -2557,38 +2598,6 @@
     <mergeCell ref="C7:E7"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="F22:H22"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A8 A10 A12 A14 A16 A18 A20 A22" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2643,38 +2652,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="123" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2686,11 +2695,11 @@
       <c r="C3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="39"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="6" t="s">
         <v>52</v>
       </c>
@@ -2711,11 +2720,11 @@
       <c r="C4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="9" t="s">
         <v>53</v>
       </c>
@@ -2736,11 +2745,11 @@
       <c r="C5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="7" t="s">
         <v>54</v>
       </c>
@@ -2755,9 +2764,9 @@
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -2770,9 +2779,9 @@
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -2785,9 +2794,9 @@
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -2800,9 +2809,9 @@
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -2815,9 +2824,9 @@
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -2830,9 +2839,9 @@
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="29"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -2845,9 +2854,9 @@
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -2860,9 +2869,9 @@
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="25"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="29"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -2875,9 +2884,9 @@
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -2890,9 +2899,9 @@
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -2905,9 +2914,9 @@
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -2920,9 +2929,9 @@
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -2935,9 +2944,9 @@
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -2950,9 +2959,9 @@
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -2965,9 +2974,9 @@
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="40"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -2980,9 +2989,9 @@
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="25"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -2995,9 +3004,9 @@
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="28"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="26"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -3010,9 +3019,9 @@
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -3023,13 +3032,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D9:F9"/>
@@ -3041,11 +3048,13 @@
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A23" xr:uid="{754EFBE9-6900-49FB-BD75-ABEDB98186B5}">
@@ -3064,7 +3073,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:M14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,38 +3098,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -3280,38 +3289,38 @@
       <c r="M11" s="7"/>
     </row>
     <row r="13" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
     </row>
     <row r="14" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
     </row>
     <row r="15" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
@@ -3349,14 +3358,14 @@
       <c r="B16" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="45">
+        <v>201</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -3501,10 +3510,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4187848-1F84-4A13-AF83-2D22DFFC9B06}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3523,38 +3532,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="A1" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -3587,19 +3596,19 @@
     </row>
     <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>53</v>
@@ -3614,25 +3623,25 @@
     </row>
     <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>54</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -3643,25 +3652,25 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
@@ -3672,25 +3681,25 @@
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -3701,25 +3710,25 @@
     </row>
     <row r="8" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -3730,25 +3739,25 @@
     </row>
     <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -3759,25 +3768,25 @@
     </row>
     <row r="10" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -3788,25 +3797,25 @@
     </row>
     <row r="11" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -3817,25 +3826,25 @@
     </row>
     <row r="12" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
@@ -3846,25 +3855,25 @@
     </row>
     <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -3875,25 +3884,25 @@
     </row>
     <row r="14" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -3904,25 +3913,25 @@
     </row>
     <row r="15" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -3933,25 +3942,25 @@
     </row>
     <row r="16" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
@@ -3962,25 +3971,25 @@
     </row>
     <row r="17" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -3991,25 +4000,25 @@
     </row>
     <row r="18" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
@@ -4020,25 +4029,25 @@
     </row>
     <row r="19" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -4049,25 +4058,25 @@
     </row>
     <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
@@ -4078,19 +4087,19 @@
     </row>
     <row r="21" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>53</v>
@@ -4105,25 +4114,25 @@
     </row>
     <row r="22" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
@@ -4134,19 +4143,19 @@
     </row>
     <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>53</v>
@@ -4161,19 +4170,19 @@
     </row>
     <row r="24" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>53</v>
@@ -4188,19 +4197,19 @@
     </row>
     <row r="25" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>53</v>
@@ -4215,24 +4224,26 @@
     </row>
     <row r="26" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="9"/>
+      <c r="G26" s="9" t="s">
+        <v>206</v>
+      </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -4242,25 +4253,25 @@
     </row>
     <row r="27" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -4271,25 +4282,25 @@
     </row>
     <row r="28" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
@@ -4300,25 +4311,25 @@
     </row>
     <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -4329,25 +4340,25 @@
     </row>
     <row r="30" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>228</v>
+        <v>174</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
@@ -4358,25 +4369,25 @@
     </row>
     <row r="31" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -4387,25 +4398,25 @@
     </row>
     <row r="32" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
@@ -4416,25 +4427,25 @@
     </row>
     <row r="33" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -4445,25 +4456,25 @@
     </row>
     <row r="34" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -4474,25 +4485,25 @@
     </row>
     <row r="35" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
@@ -4503,25 +4514,25 @@
     </row>
     <row r="36" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
@@ -4532,25 +4543,25 @@
     </row>
     <row r="37" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
@@ -4561,25 +4572,25 @@
     </row>
     <row r="38" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>53</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -4590,25 +4601,25 @@
     </row>
     <row r="39" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
@@ -4617,51 +4628,22 @@
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
     </row>
-    <row r="40" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="B2:M2"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type Error" error="Options for Adding Bridge Domain is add_bd or nca_bd" sqref="A4:A40" xr:uid="{73607855-EC72-4AF6-9FDA-5A5C0A35C0B4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Type Error" error="Options for Adding Bridge Domain is add_bd or nca_bd" sqref="A4:A39" xr:uid="{73607855-EC72-4AF6-9FDA-5A5C0A35C0B4}">
       <formula1>"add_bd,nca_bd"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F40" xr:uid="{FA86EA4B-6A0D-4C04-B3DC-114E5FC0F4E7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F39" xr:uid="{FA86EA4B-6A0D-4C04-B3DC-114E5FC0F4E7}">
       <formula1>"pg,vzAny,neither"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Extend Outside ACI" error="Valid answers are no or yes" sqref="E4:E40" xr:uid="{DB07E8DF-D953-415E-99BF-BA6F30509808}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Extend Outside ACI" error="Valid answers are no or yes" sqref="E4:E39" xr:uid="{DB07E8DF-D953-415E-99BF-BA6F30509808}">
       <formula1>"no,yes"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B4:B40" xr:uid="{7940DCC3-9A19-4E58-9369-0FFBAFD24953}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B4:B39" xr:uid="{7940DCC3-9A19-4E58-9369-0FFBAFD24953}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -4698,38 +4680,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -4933,38 +4915,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -4982,11 +4964,11 @@
       <c r="E3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -5009,9 +4991,9 @@
       <c r="E4" s="10">
         <v>202</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -5024,9 +5006,9 @@
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -5039,9 +5021,9 @@
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -5054,9 +5036,9 @@
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -5069,9 +5051,9 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -5084,9 +5066,9 @@
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -5099,9 +5081,9 @@
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -5110,16 +5092,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B4:B10" xr:uid="{0E2C46BF-216F-49C7-A16B-609641BE53B2}">
@@ -5147,7 +5129,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5172,38 +5154,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
     </row>
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -5221,11 +5203,11 @@
       <c r="E3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -5248,9 +5230,9 @@
       <c r="E4" s="10">
         <v>202</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -5263,9 +5245,9 @@
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -5278,9 +5260,9 @@
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
@@ -5293,9 +5275,9 @@
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -5308,9 +5290,9 @@
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -5323,9 +5305,9 @@
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -5338,9 +5320,9 @@
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -5385,25 +5367,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC9172D-5165-4643-8D6D-406EE90B9A46}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" style="4" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="39.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="34.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" style="4" customWidth="1"/>
     <col min="15" max="15" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -5414,78 +5396,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
+      <c r="A1" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
     </row>
     <row r="2" spans="1:19" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
     </row>
     <row r="3" spans="1:19" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -5502,10 +5484,10 @@
     </row>
     <row r="4" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>2</v>
@@ -5526,7 +5508,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
@@ -5645,365 +5627,365 @@
       <c r="S9" s="13"/>
     </row>
     <row r="11" spans="1:19" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="40"/>
-      <c r="S11" s="40"/>
+      <c r="A11" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
     </row>
     <row r="12" spans="1:19" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="41"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="42"/>
+      <c r="N12" s="42"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
     </row>
     <row r="13" spans="1:19" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="I13" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="O13" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="K13" s="6" t="s">
+      <c r="P13" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="Q13" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="R13" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="S13" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="S13" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>246</v>
+        <v>238</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>233</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H14" s="12">
         <v>1</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="43">
+        <v>1500</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="43">
+        <v>1</v>
+      </c>
+      <c r="M14" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L14" s="12" t="s">
+      <c r="N14" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q14" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="R14" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="S14" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="N14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="P14" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q14" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="R14" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="S14" s="12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>246</v>
+        <v>239</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>233</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H15" s="13">
         <v>1</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="44">
+        <v>1500</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" s="44">
+        <v>1</v>
+      </c>
+      <c r="M15" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="J15" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="M15" s="13" t="s">
+      <c r="N15" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q15" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="R15" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="N15" s="13" t="s">
+      <c r="S15" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="O15" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="P15" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q15" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="R15" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="S15" s="13" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C16" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="D16" s="46">
+        <v>201</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D16" s="7">
-        <v>201</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>165</v>
-      </c>
       <c r="F16" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H16" s="12">
         <v>1</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>77</v>
+      <c r="I16" s="43">
+        <v>1500</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="L16" s="43">
+        <v>995</v>
       </c>
       <c r="M16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="P16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q16" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="R16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="S16" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="N16" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q16" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="S16" s="12" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D17" s="9">
+        <v>241</v>
+      </c>
+      <c r="D17" s="47">
         <v>201</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H17" s="13">
         <v>1</v>
       </c>
-      <c r="I17" s="17" t="s">
-        <v>77</v>
+      <c r="I17" s="44">
+        <v>1500</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="L17" s="44">
+        <v>995</v>
       </c>
       <c r="M17" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O17" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P17" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q17" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R17" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="S17" s="13"/>
     </row>
     <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>246</v>
+        <v>125</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>233</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H18" s="12">
         <v>1</v>
@@ -6012,55 +5994,55 @@
         <v>9000</v>
       </c>
       <c r="J18" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K18" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="L18" s="43">
+        <v>691</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="R18" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="N18" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="R18" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="S18" s="12"/>
     </row>
     <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B19" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>246</v>
+        <v>126</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>233</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H19" s="13">
         <v>1</v>
@@ -6069,112 +6051,112 @@
         <v>9000</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>90</v>
+        <v>83</v>
+      </c>
+      <c r="L19" s="44">
+        <v>691</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O19" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q19" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R19" s="13" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="S19" s="13"/>
     </row>
     <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="7">
+        <v>127</v>
+      </c>
+      <c r="D20" s="46">
         <v>201</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H20" s="12">
         <v>1</v>
       </c>
-      <c r="I20" s="16" t="s">
-        <v>77</v>
+      <c r="I20" s="43">
+        <v>1500</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="L20" s="12">
+        <v>83</v>
+      </c>
+      <c r="L20" s="16">
         <v>691</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R20" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="S20" s="12"/>
     </row>
     <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>246</v>
+        <v>128</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>233</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H21" s="13">
         <v>1</v>
@@ -6183,55 +6165,55 @@
         <v>9000</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L21" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L21" s="44">
+        <v>1</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O21" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q21" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R21" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="S21" s="13"/>
     </row>
     <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>246</v>
+        <v>129</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>233</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H22" s="12">
         <v>1</v>
@@ -6240,55 +6222,55 @@
         <v>9000</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L22" s="43">
+        <v>1</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N22" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q22" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R22" s="12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="S22" s="12"/>
     </row>
     <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>127</v>
+        <v>130</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>235</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H23" s="13">
         <v>1</v>
@@ -6297,55 +6279,55 @@
         <v>9000</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L23" s="44">
+        <v>1</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O23" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q23" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R23" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>246</v>
+        <v>131</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>233</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H24" s="12">
         <v>1</v>
@@ -6354,57 +6336,57 @@
         <v>9000</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L24" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L24" s="43">
+        <v>1</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O24" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R24" s="12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="S24" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>246</v>
+        <v>132</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>233</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H25" s="13">
         <v>1</v>
@@ -6413,57 +6395,57 @@
         <v>9000</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L25" s="44">
+        <v>1</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O25" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q25" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R25" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="S25" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>246</v>
+        <v>133</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>233</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H26" s="12">
         <v>1</v>
@@ -6472,55 +6454,55 @@
         <v>9000</v>
       </c>
       <c r="J26" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L26" s="43">
+        <v>1</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O26" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P26" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q26" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R26" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="S26" s="12"/>
     </row>
     <row r="27" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B27" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>246</v>
+        <v>134</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>233</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H27" s="13">
         <v>1</v>
@@ -6529,55 +6511,55 @@
         <v>9000</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L27" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L27" s="44">
+        <v>1</v>
       </c>
       <c r="M27" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O27" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P27" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q27" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R27" s="13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>130</v>
+        <v>135</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>236</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H28" s="12">
         <v>1</v>
@@ -6586,55 +6568,55 @@
         <v>9000</v>
       </c>
       <c r="J28" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L28" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L28" s="43">
+        <v>1</v>
       </c>
       <c r="M28" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N28" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O28" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q28" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R28" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="S28" s="12"/>
     </row>
     <row r="29" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>130</v>
+        <v>136</v>
+      </c>
+      <c r="D29" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>236</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H29" s="13">
         <v>1</v>
@@ -6643,55 +6625,55 @@
         <v>9000</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L29" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L29" s="44">
+        <v>1</v>
       </c>
       <c r="M29" s="13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N29" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O29" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P29" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q29" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R29" s="13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="S29" s="13"/>
     </row>
     <row r="30" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>131</v>
+        <v>137</v>
+      </c>
+      <c r="D30" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>237</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H30" s="12">
         <v>1</v>
@@ -6700,55 +6682,55 @@
         <v>9000</v>
       </c>
       <c r="J30" s="12" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L30" s="43">
+        <v>1</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N30" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O30" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P30" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q30" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R30" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="S30" s="12"/>
     </row>
     <row r="31" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>131</v>
+        <v>138</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="H31" s="13">
         <v>1</v>
@@ -6757,31 +6739,31 @@
         <v>9000</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L31" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="L31" s="44">
+        <v>1</v>
       </c>
       <c r="M31" s="13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N31" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O31" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="P31" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q31" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="R31" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="S31" s="13"/>
     </row>
@@ -6860,13 +6842,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6907,7 +6889,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -6952,7 +6934,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6961,7 +6943,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6970,7 +6952,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -6979,7 +6961,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>